<commit_message>
Fu Wu Zhong Xin
</commit_message>
<xml_diff>
--- a/activity/计划.xlsx
+++ b/activity/计划.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12465"/>
+    <workbookView windowWidth="28800" windowHeight="12465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="网页" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,18 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
-  <si>
-    <t>序号</t>
-  </si>
-  <si>
-    <t>内   容</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
+  <si>
+    <t>计划编号</t>
+  </si>
+  <si>
+    <t>计划标题</t>
   </si>
   <si>
     <t>责任部门/人</t>
   </si>
   <si>
-    <t>计划完成时间</t>
+    <t>预计完成时间</t>
+  </si>
+  <si>
+    <t>计划状态</t>
   </si>
   <si>
     <t>备注</t>
@@ -39,12 +42,18 @@
     <t>客服部</t>
   </si>
   <si>
+    <t>进行中</t>
+  </si>
+  <si>
     <t>小区总水、电表费用结算并过户</t>
   </si>
   <si>
     <t>整理规范所有小区分包方和供应商，签订合同（电梯、消防、清洁等）</t>
   </si>
   <si>
+    <t>已完成</t>
+  </si>
+  <si>
     <t>组织全面清理楼道及公共区域大件垃圾，改善小区卫生环境</t>
   </si>
   <si>
@@ -72,6 +81,9 @@
     <t>启动节能水泵改造评估</t>
   </si>
   <si>
+    <t>未开始</t>
+  </si>
+  <si>
     <t>全面恢复小区门禁系统</t>
   </si>
   <si>
@@ -79,6 +91,21 @@
   </si>
   <si>
     <t>全面恢复监控系统</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;td scope="row" data-label="商谈问题"&gt;新老物业交接时间&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;td data-label="金岸物业"&gt;未表态&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;td data-label="业委会意见"&gt;业委会已发函告知业主，金岸物业，开发商，工作站，街道办，住建局，派出所等单位，新老物业交接的时间是2018年11月30号早上9点整。&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;td data-label="商谈结果"&gt;待金岸物业明确回复&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;/tr&gt;</t>
   </si>
 </sst>
 </file>
@@ -86,20 +113,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,154 +577,160 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1057,22 +1083,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="10.375" customWidth="1"/>
     <col min="2" max="2" width="65" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="35.75" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
+    <col min="6" max="6" width="35.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1088,258 +1115,325 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
-        <v>1</v>
+        <v>20181215</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3">
         <v>43600</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
-        <v>2</v>
+        <v>20181216</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>43495</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
-        <v>3</v>
+        <v>20181217</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3">
+        <v>43495</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>20181218</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3">
+        <v>43524</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>20181219</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3">
+        <v>43485</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>20181220</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3">
         <v>43495</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1">
-        <v>43524</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1">
-        <v>43485</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>20181221</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3">
         <v>43495</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>20181222</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3">
         <v>43495</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>20181223</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3">
         <v>43495</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1">
-        <v>43495</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
-        <v>10</v>
+        <v>20181224</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3">
         <v>43475</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
-        <v>11</v>
+        <v>20181225</v>
       </c>
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>43496</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
-        <v>12</v>
+        <v>20181226</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="1">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3">
         <v>43496</v>
       </c>
-    </row>
-    <row r="14" spans="4:4">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="4:4">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="4:4">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="4:4">
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="4:4">
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="4:4">
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="4:4">
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="4:4">
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="4:4">
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="4:4">
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="4:4">
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="4:4">
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="4:4">
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="4:4">
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="4:4">
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="4:4">
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="4:4">
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="4:4">
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="4:4">
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="4:4">
-      <c r="D41" s="1"/>
+      <c r="E13" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="4:5">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="4:5">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="4:5">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="4:5">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="4:5">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="4:5">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="4:5">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="4:5">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="4:5">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="4:5">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="4:5">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="4:5">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="4:5">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="4:5">
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="4:5">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="4:5">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="4:5">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="4:5">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="4:5">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="4:5">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="4:5">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="4:5">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="4:5">
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="4:5">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="4:5">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1351,14 +1445,61 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="C2:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
+  <cols>
+    <col min="3" max="3" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" ht="409.5" spans="3:3">
+      <c r="C2" s="2" t="str">
+        <f>"&lt;tr&gt;
+&lt;td data-label="""&amp;Sheet1!$A$1&amp;"""&gt;"&amp;Sheet1!$A2&amp;"&lt;/td&gt;
+&lt;td data-label="""&amp;Sheet1!$B$1&amp;"""&gt;"&amp;Sheet1!$B2&amp;"&lt;/td&gt;
+&lt;td data-label="""&amp;Sheet1!$C$1&amp;"""&gt;"&amp;Sheet1!$C2&amp;"&lt;/td&gt;
+&lt;td data-label="""&amp;Sheet1!$D$1&amp;"""&gt;"&amp;Sheet1!$D2&amp;"&lt;/td&gt;
+&lt;td data-label="""&amp;Sheet1!$E$1&amp;"""&gt;"&amp;Sheet1!$E2&amp;"&lt;/td&gt;
+&lt;/tr&gt;"</f>
+        <v>&lt;tr&gt;
+&lt;td data-label="计划编号"&gt;20181215&lt;/td&gt;
+&lt;td data-label="计划标题"&gt;建立业主档案和银行账户托收协议的办理&lt;/td&gt;
+&lt;td data-label="责任部门/人"&gt;客服部&lt;/td&gt;
+&lt;td data-label="预计完成时间"&gt;43600&lt;/td&gt;
+&lt;td data-label="计划状态"&gt;进行中&lt;/td&gt;
+&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="10:10">
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="10:10">
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="10:10">
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="10:10">
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="10:10">
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>